<commit_message>
stevan App IOS Automation
</commit_message>
<xml_diff>
--- a/src/test/java/com/forrester/xls/TestCasesForrester.xlsx
+++ b/src/test/java/com/forrester/xls/TestCasesForrester.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>TCID</t>
   </si>
@@ -89,31 +89,31 @@
     <t>Results</t>
   </si>
   <si>
+    <t>ExpectedText</t>
+  </si>
+  <si>
+    <t>Bon</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Mobs</t>
+  </si>
+  <si>
+    <t>Phil</t>
+  </si>
+  <si>
+    <t>Tex</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>ExpectedText</t>
-  </si>
-  <si>
-    <t>Bon</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Mobs</t>
-  </si>
-  <si>
-    <t>Phil</t>
-  </si>
-  <si>
-    <t>Tex</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Skipped</t>
   </si>
 </sst>
 </file>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -564,7 +564,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -578,7 +578,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -592,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -606,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -676,10 +676,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>14</v>
@@ -715,7 +715,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -726,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -737,12 +737,12 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId70" display="its.thakur@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId26" display="its.thakur@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>